<commit_message>
CCDD-35 Aquisição - IDEB (#12)
* faz rename dos arquivos

* cria ETL do IDEB

* organiza comandos de processamento

* ajusta o processamento do IDEB

* ajusta configurações

* cria o teste unitário do IDEB

* deleta notebooks de exploração

* ajusta fixtures dos testes

* mypy e otimiza imports

* ajusta teste ideb e zona residencial

* black e otimiza imports

* remove cache

Co-authored-by: Pedro Forli <pedro.henrique.forli@gmail.com>
</commit_message>
<xml_diff>
--- a/src/info/aquis_censo_docentes_cols.xlsx
+++ b/src/info/aquis_censo_docentes_cols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro.forli\PycharmProjects\curso-ciencia-dados\src\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C149016-EAC3-4A9B-85FF-1651FB8D94D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711E7512-86A0-480D-A95F-87423AC390EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48C7DDBA-442F-4222-8A07-8EDC411B5A7F}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="310">
   <si>
     <t>NU_ANO_CENSO</t>
   </si>
@@ -990,6 +990,9 @@
   </si>
   <si>
     <t>IN_INTERCULTURAL_OUTROS</t>
+  </si>
+  <si>
+    <t>ID_ESCOLA</t>
   </si>
 </sst>
 </file>
@@ -1529,7 +1532,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70D7738B-264F-484F-BE6D-FD3693129414}">
   <dimension ref="A1:C287"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2833,7 +2838,7 @@
         <v>33</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>5</v>
+        <v>309</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -4307,7 +4312,7 @@
         <v>33</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>5</v>
+        <v>309</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>